<commit_message>
feat: add new evaluation algorithm.
</commit_message>
<xml_diff>
--- a/spreadsheets/Holiday budget planner.xlsx
+++ b/spreadsheets/Holiday budget planner.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB91923-514A-4C98-8E87-A79F90E0F7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1323BC-ACB1-4371-9FE7-2ABA2151E2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10410" yWindow="3180" windowWidth="17800" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7470" yWindow="2980" windowWidth="21760" windowHeight="13400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Holiday budget planner" sheetId="1" r:id="rId1"/>
@@ -719,11 +719,6 @@
   <dxfs count="87">
     <dxf>
       <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -799,7 +794,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -808,6 +803,402 @@
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -851,11 +1242,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
+        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -888,6 +1275,38 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="8" tint="-0.249977111117893"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
       <fill>
         <patternFill patternType="none">
@@ -899,11 +1318,7 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
+        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -924,6 +1339,32 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -947,11 +1388,51 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -971,8 +1452,171 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
+      <border>
+        <top style="hair">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -992,13 +1636,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
-          <color theme="8" tint="-0.249977111117893"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1026,7 +1663,11 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1047,13 +1688,6 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="4" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1074,17 +1708,13 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
         <name val="Tw Cen MT"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1096,15 +1726,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="hair">
-          <color theme="0" tint="-0.499984740745262"/>
-        </top>
-        <bottom/>
-      </border>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1130,17 +1752,13 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
         <name val="Tw Cen MT"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1152,15 +1770,101 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
         <top style="hair">
           <color theme="0" tint="-0.499984740745262"/>
         </top>
-        <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color theme="4" tint="-0.249977111117893"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Tw Cen MT"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1186,17 +1890,13 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
         <name val="Tw Cen MT"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -1208,15 +1908,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="hair">
-          <color theme="0" tint="-0.499984740745262"/>
-        </top>
-        <bottom/>
-      </border>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1239,783 +1931,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top style="hair">
-          <color theme="0" tint="-0.499984740745262"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="hair">
-          <color theme="0" tint="-0.499984740745262"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="4" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="hair">
-          <color theme="0" tint="-0.499984740745262"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color theme="4" tint="-0.249977111117893"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Tw Cen MT"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2466,10 +2381,14 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="71" totalsRowDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Budget" totalsRowFunction="sum" dataDxfId="70" totalsRowDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Actual" totalsRowFunction="sum" dataDxfId="69" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Difference" totalsRowFunction="sum" dataDxfId="68" totalsRowDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="71" totalsRowDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Budget" totalsRowFunction="custom" dataDxfId="70" totalsRowDxfId="22">
+      <totalsRowFormula>SUM(Gifts[Budget])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Actual" totalsRowFunction="custom" dataDxfId="69" totalsRowDxfId="21">
+      <totalsRowFormula>SUM(Gifts[Actual])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Difference" totalsRowFunction="sum" dataDxfId="68" totalsRowDxfId="20">
       <calculatedColumnFormula>Gifts[[#This Row],[Budget]]-Gifts[[#This Row],[Actual]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2483,18 +2402,22 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Packaging" displayName="Packaging" ref="C19:F27" totalsRowCount="1" headerRowDxfId="67" dataDxfId="65" totalsRowDxfId="64" headerRowBorderDxfId="66" totalsRowBorderDxfId="63">
-  <autoFilter ref="C19:F26" xr:uid="{00000000-0009-0000-0100-000004000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Packaging" displayName="Packaging" ref="C20:F28" totalsRowCount="1" headerRowDxfId="67" dataDxfId="65" totalsRowDxfId="64" headerRowBorderDxfId="66" totalsRowBorderDxfId="63">
+  <autoFilter ref="C20:F27" xr:uid="{00000000-0009-0000-0100-000004000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="62" totalsRowDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Budget" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Actual" totalsRowFunction="sum" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Difference" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="55">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="62" totalsRowDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Budget" totalsRowFunction="custom" dataDxfId="61" totalsRowDxfId="14">
+      <totalsRowFormula>SUM(Packaging[Budget])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Actual" totalsRowFunction="custom" dataDxfId="60" totalsRowDxfId="13">
+      <totalsRowFormula>SUM(Packaging[Actual])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Difference" totalsRowFunction="sum" dataDxfId="59" totalsRowDxfId="12">
       <calculatedColumnFormula>Packaging[[#This Row],[Budget]]-Packaging[[#This Row],[Actual]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2508,18 +2431,22 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Entertainment" displayName="Entertainment" ref="K19:N27" totalsRowCount="1" headerRowDxfId="54" dataDxfId="52" totalsRowDxfId="51" headerRowBorderDxfId="53" totalsRowBorderDxfId="50">
-  <autoFilter ref="K19:N26" xr:uid="{00000000-0009-0000-0100-000005000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Entertainment" displayName="Entertainment" ref="K20:N28" totalsRowCount="1" headerRowDxfId="58" dataDxfId="56" totalsRowDxfId="55" headerRowBorderDxfId="57" totalsRowBorderDxfId="54">
+  <autoFilter ref="K20:N27" xr:uid="{00000000-0009-0000-0100-000005000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Budget" totalsRowFunction="sum" dataDxfId="47" totalsRowDxfId="46"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Actual" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Difference" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="53" totalsRowDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Budget" totalsRowFunction="custom" dataDxfId="52" totalsRowDxfId="10">
+      <totalsRowFormula>SUM(Entertainment[Budget])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Actual" totalsRowFunction="custom" dataDxfId="51" totalsRowDxfId="9">
+      <totalsRowFormula>SUM(Entertainment[Actual])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Difference" totalsRowFunction="sum" dataDxfId="50" totalsRowDxfId="8">
       <calculatedColumnFormula>Entertainment[[#This Row],[Budget]]-Entertainment[[#This Row],[Actual]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2533,18 +2460,22 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Miscellaneous" displayName="Miscellaneous" ref="K29:N34" totalsRowCount="1" headerRowDxfId="41" dataDxfId="40" totalsRowDxfId="39">
-  <autoFilter ref="K29:N33" xr:uid="{00000000-0009-0000-0100-000007000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Miscellaneous" displayName="Miscellaneous" ref="K31:N36" totalsRowCount="1" headerRowDxfId="49" dataDxfId="48" totalsRowDxfId="47">
+  <autoFilter ref="K31:N35" xr:uid="{00000000-0009-0000-0100-000007000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Budget" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Actual" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Difference" totalsRowFunction="sum" dataDxfId="32" totalsRowDxfId="31">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="46" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Budget" totalsRowFunction="custom" dataDxfId="45" totalsRowDxfId="2">
+      <totalsRowFormula>SUM(Miscellaneous[Budget])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Actual" totalsRowFunction="custom" dataDxfId="44" totalsRowDxfId="1">
+      <totalsRowFormula>SUM(Miscellaneous[Actual])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Difference" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="0">
       <calculatedColumnFormula>Miscellaneous[[#This Row],[Budget]]-Miscellaneous[[#This Row],[Actual]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2558,18 +2489,22 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Travel" displayName="Travel" ref="C29:F34" totalsRowCount="1" headerRowDxfId="30" dataDxfId="28" totalsRowDxfId="27" headerRowBorderDxfId="29" totalsRowBorderDxfId="26">
-  <autoFilter ref="C29:F33" xr:uid="{00000000-0009-0000-0100-000006000000}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Travel" displayName="Travel" ref="C31:F36" totalsRowCount="1" headerRowDxfId="42" dataDxfId="40" totalsRowDxfId="39" headerRowBorderDxfId="41" totalsRowBorderDxfId="38">
+  <autoFilter ref="C31:F35" xr:uid="{00000000-0009-0000-0100-000006000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Budget" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Actual" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Difference" totalsRowFunction="sum" dataDxfId="19" totalsRowDxfId="18">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="37" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Budget" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="6">
+      <totalsRowFormula>SUM(Travel[Budget])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Actual" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="5">
+      <totalsRowFormula>SUM(Travel[Actual])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="Difference" totalsRowFunction="sum" dataDxfId="34" totalsRowDxfId="4">
       <calculatedColumnFormula>Travel[[#This Row],[Budget]]-Travel[[#This Row],[Actual]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2583,7 +2518,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Meals" displayName="Meals" ref="K10:N17" totalsRowCount="1" headerRowDxfId="17" dataDxfId="15" totalsRowDxfId="14" headerRowBorderDxfId="16" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Meals" displayName="Meals" ref="K10:N17" totalsRowCount="1" headerRowDxfId="33" dataDxfId="31" totalsRowDxfId="30" headerRowBorderDxfId="32" totalsRowBorderDxfId="29">
   <autoFilter ref="K10:N16" xr:uid="{00000000-0009-0000-0100-000002000000}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -2591,10 +2526,14 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Budget" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Actual" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Difference" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Item" totalsRowLabel="Total" dataDxfId="28" totalsRowDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Budget" totalsRowFunction="custom" dataDxfId="27" totalsRowDxfId="18">
+      <totalsRowFormula>SUM(Meals[Budget])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Actual" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="17">
+      <totalsRowFormula>SUM(Meals[Actual])</totalsRowFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Difference" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="16">
       <calculatedColumnFormula>Meals[[#This Row],[Budget]]-Meals[[#This Row],[Actual]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2898,10 +2837,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -3050,7 +2989,7 @@
       <c r="L6" s="26"/>
       <c r="M6" s="44"/>
       <c r="N6" s="27">
-        <f>SUM(N3-N4)</f>
+        <f>N3-N4</f>
         <v>-70</v>
       </c>
       <c r="O6" s="19"/>
@@ -3319,11 +3258,11 @@
         <v>19</v>
       </c>
       <c r="D17" s="32">
-        <f>SUBTOTAL(109,Gifts[Budget])</f>
+        <f>SUM(Gifts[Budget])</f>
         <v>750</v>
       </c>
       <c r="E17" s="32">
-        <f>SUBTOTAL(109,Gifts[Actual])</f>
+        <f>SUM(Gifts[Actual])</f>
         <v>820</v>
       </c>
       <c r="F17" s="32">
@@ -3338,11 +3277,11 @@
         <v>19</v>
       </c>
       <c r="L17" s="32">
-        <f>SUBTOTAL(109,Meals[Budget])</f>
+        <f>SUM(Meals[Budget])</f>
         <v>0</v>
       </c>
       <c r="M17" s="32">
-        <f>SUBTOTAL(109,Meals[Actual])</f>
+        <f>SUM(Meals[Actual])</f>
         <v>0</v>
       </c>
       <c r="N17" s="32">
@@ -3351,89 +3290,79 @@
       </c>
       <c r="O17" s="52"/>
     </row>
-    <row r="18" spans="1:15" s="48" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18"/>
+    <row r="18" spans="1:15" s="48" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="16"/>
-      <c r="C18" s="66" t="s">
+      <c r="C18" s="36"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="52"/>
+    </row>
+    <row r="19" spans="1:15" s="48" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="61" t="s">
+      <c r="D19" s="66"/>
+      <c r="E19" s="66"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="L18" s="61"/>
-      <c r="M18" s="61"/>
-      <c r="N18" s="61"/>
-      <c r="O18" s="30"/>
+      <c r="L19" s="61"/>
+      <c r="M19" s="61"/>
+      <c r="N19" s="61"/>
+      <c r="O19" s="30"/>
     </row>
-    <row r="19" spans="1:15" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="17"/>
-      <c r="C19" s="33" t="s">
+    <row r="20" spans="1:15" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="17"/>
+      <c r="C20" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="37" t="s">
+      <c r="D20" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="37" t="s">
+      <c r="E20" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="37" t="s">
+      <c r="F20" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G19" s="49"/>
-      <c r="H19" s="50"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="33" t="s">
+      <c r="G20" s="49"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="L19" s="37" t="s">
+      <c r="L20" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="M19" s="37" t="s">
+      <c r="M20" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="N19" s="37" t="s">
+      <c r="N20" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="O19" s="49"/>
-    </row>
-    <row r="20" spans="1:15" s="48" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="16"/>
-      <c r="C20" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32">
-        <f>Packaging[[#This Row],[Budget]]-Packaging[[#This Row],[Actual]]</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="31"/>
-      <c r="H20" s="51"/>
-      <c r="I20" s="51"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32">
-        <f>Entertainment[[#This Row],[Budget]]-Entertainment[[#This Row],[Actual]]</f>
-        <v>0</v>
-      </c>
-      <c r="O20" s="32"/>
+      <c r="O20" s="49"/>
     </row>
     <row r="21" spans="1:15" s="48" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="16"/>
       <c r="C21" s="36" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D21" s="32"/>
       <c r="E21" s="32"/>
@@ -3446,7 +3375,7 @@
       <c r="I21" s="51"/>
       <c r="J21" s="12"/>
       <c r="K21" s="36" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="L21" s="32"/>
       <c r="M21" s="32"/>
@@ -3459,7 +3388,7 @@
     <row r="22" spans="1:15" s="48" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="16"/>
       <c r="C22" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="32"/>
       <c r="E22" s="32"/>
@@ -3472,7 +3401,7 @@
       <c r="I22" s="51"/>
       <c r="J22" s="12"/>
       <c r="K22" s="36" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="L22" s="32"/>
       <c r="M22" s="32"/>
@@ -3485,7 +3414,7 @@
     <row r="23" spans="1:15" s="48" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="16"/>
       <c r="C23" s="36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D23" s="32"/>
       <c r="E23" s="32"/>
@@ -3498,7 +3427,7 @@
       <c r="I23" s="51"/>
       <c r="J23" s="12"/>
       <c r="K23" s="36" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L23" s="32"/>
       <c r="M23" s="32"/>
@@ -3511,7 +3440,7 @@
     <row r="24" spans="1:15" s="48" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="16"/>
       <c r="C24" s="36" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D24" s="32"/>
       <c r="E24" s="32"/>
@@ -3524,7 +3453,7 @@
       <c r="I24" s="51"/>
       <c r="J24" s="12"/>
       <c r="K24" s="36" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L24" s="32"/>
       <c r="M24" s="32"/>
@@ -3537,7 +3466,7 @@
     <row r="25" spans="1:15" s="48" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="16"/>
       <c r="C25" s="36" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D25" s="32"/>
       <c r="E25" s="32"/>
@@ -3550,7 +3479,7 @@
       <c r="I25" s="51"/>
       <c r="J25" s="12"/>
       <c r="K25" s="36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L25" s="32"/>
       <c r="M25" s="32"/>
@@ -3571,12 +3500,12 @@
         <f>Packaging[[#This Row],[Budget]]-Packaging[[#This Row],[Actual]]</f>
         <v>0</v>
       </c>
-      <c r="G26" s="34"/>
+      <c r="G26" s="31"/>
       <c r="H26" s="51"/>
       <c r="I26" s="51"/>
       <c r="J26" s="12"/>
       <c r="K26" s="36" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="L26" s="32"/>
       <c r="M26" s="32"/>
@@ -3586,152 +3515,142 @@
       </c>
       <c r="O26" s="32"/>
     </row>
-    <row r="27" spans="1:15" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" s="48" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="16"/>
-      <c r="C27" s="33" t="s">
+      <c r="C27" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32">
+        <f>Packaging[[#This Row],[Budget]]-Packaging[[#This Row],[Actual]]</f>
+        <v>0</v>
+      </c>
+      <c r="G27" s="34"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32">
+        <f>Entertainment[[#This Row],[Budget]]-Entertainment[[#This Row],[Actual]]</f>
+        <v>0</v>
+      </c>
+      <c r="O27" s="32"/>
+    </row>
+    <row r="28" spans="1:15" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="16"/>
+      <c r="C28" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="32">
-        <f>SUBTOTAL(109,Packaging[Budget])</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="32">
-        <f>SUBTOTAL(109,Packaging[Actual])</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="32">
+      <c r="D28" s="32">
+        <f>SUM(Packaging[Budget])</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="32">
+        <f>SUM(Packaging[Actual])</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="32">
         <f>SUBTOTAL(109,Packaging[Difference])</f>
         <v>0</v>
       </c>
-      <c r="G27" s="52"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
-      <c r="J27" s="53"/>
-      <c r="K27" s="33" t="s">
+      <c r="G28" s="52"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L27" s="32">
-        <f>SUBTOTAL(109,Entertainment[Budget])</f>
-        <v>0</v>
-      </c>
-      <c r="M27" s="32">
-        <f>SUBTOTAL(109,Entertainment[Actual])</f>
-        <v>0</v>
-      </c>
-      <c r="N27" s="32">
+      <c r="L28" s="32">
+        <f>SUM(Entertainment[Budget])</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="32">
+        <f>SUM(Entertainment[Actual])</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="32">
         <f>SUBTOTAL(109,Entertainment[Difference])</f>
         <v>0</v>
       </c>
-      <c r="O27" s="35"/>
+      <c r="O28" s="35"/>
     </row>
-    <row r="28" spans="1:15" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="16"/>
-      <c r="C28" s="62" t="s">
+    <row r="29" spans="1:15" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="16"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="52"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="K29" s="33"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
+      <c r="O29" s="35"/>
+    </row>
+    <row r="30" spans="1:15" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="16"/>
+      <c r="C30" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="14"/>
-      <c r="K28" s="59" t="s">
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="30"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="L28" s="60"/>
-      <c r="M28" s="60"/>
-      <c r="N28" s="60"/>
-      <c r="O28" s="30"/>
+      <c r="L30" s="60"/>
+      <c r="M30" s="60"/>
+      <c r="N30" s="60"/>
+      <c r="O30" s="30"/>
     </row>
-    <row r="29" spans="1:15" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="16"/>
-      <c r="C29" s="33" t="s">
+    <row r="31" spans="1:15" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="16"/>
+      <c r="C31" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="37" t="s">
+      <c r="D31" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="37" t="s">
+      <c r="E31" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F29" s="37" t="s">
+      <c r="F31" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G29" s="49"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="53"/>
-      <c r="K29" s="33" t="s">
+      <c r="G31" s="49"/>
+      <c r="H31" s="50"/>
+      <c r="I31" s="50"/>
+      <c r="J31" s="53"/>
+      <c r="K31" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="L29" s="37" t="s">
+      <c r="L31" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="M29" s="37" t="s">
+      <c r="M31" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="N29" s="37" t="s">
+      <c r="N31" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="O29" s="49"/>
-    </row>
-    <row r="30" spans="1:15" s="48" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="16"/>
-      <c r="C30" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32">
-        <f>Travel[[#This Row],[Budget]]-Travel[[#This Row],[Actual]]</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="32"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="L30" s="32"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="32">
-        <f>Miscellaneous[[#This Row],[Budget]]-Miscellaneous[[#This Row],[Actual]]</f>
-        <v>0</v>
-      </c>
-      <c r="O30" s="32"/>
-    </row>
-    <row r="31" spans="1:15" s="48" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="16"/>
-      <c r="C31" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="32"/>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32">
-        <f>Travel[[#This Row],[Budget]]-Travel[[#This Row],[Actual]]</f>
-        <v>0</v>
-      </c>
-      <c r="G31" s="32"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="L31" s="32"/>
-      <c r="M31" s="32"/>
-      <c r="N31" s="32">
-        <f>Miscellaneous[[#This Row],[Budget]]-Miscellaneous[[#This Row],[Actual]]</f>
-        <v>0</v>
-      </c>
-      <c r="O31" s="32"/>
+      <c r="O31" s="49"/>
     </row>
     <row r="32" spans="1:15" s="48" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="16"/>
       <c r="C32" s="36" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D32" s="32"/>
       <c r="E32" s="32"/>
@@ -3744,7 +3663,7 @@
       <c r="I32" s="51"/>
       <c r="J32" s="12"/>
       <c r="K32" s="36" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="L32" s="32"/>
       <c r="M32" s="32"/>
@@ -3757,7 +3676,7 @@
     <row r="33" spans="2:15" s="48" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="16"/>
       <c r="C33" s="36" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D33" s="32"/>
       <c r="E33" s="32"/>
@@ -3770,7 +3689,7 @@
       <c r="I33" s="51"/>
       <c r="J33" s="12"/>
       <c r="K33" s="36" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L33" s="32"/>
       <c r="M33" s="32"/>
@@ -3778,60 +3697,112 @@
         <f>Miscellaneous[[#This Row],[Budget]]-Miscellaneous[[#This Row],[Actual]]</f>
         <v>0</v>
       </c>
-      <c r="O33" s="34"/>
+      <c r="O33" s="32"/>
     </row>
-    <row r="34" spans="2:15" s="48" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:15" s="48" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="16"/>
-      <c r="C34" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="32">
-        <f>SUBTOTAL(109,Travel[Budget])</f>
-        <v>0</v>
-      </c>
-      <c r="E34" s="32">
-        <f>SUBTOTAL(109,Travel[Actual])</f>
-        <v>0</v>
-      </c>
+      <c r="C34" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
       <c r="F34" s="32">
-        <f>SUBTOTAL(109,Travel[Difference])</f>
-        <v>0</v>
-      </c>
-      <c r="G34" s="52"/>
+        <f>Travel[[#This Row],[Budget]]-Travel[[#This Row],[Actual]]</f>
+        <v>0</v>
+      </c>
+      <c r="G34" s="32"/>
       <c r="H34" s="51"/>
       <c r="I34" s="51"/>
       <c r="J34" s="12"/>
-      <c r="K34" s="33" t="s">
+      <c r="K34" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32">
+        <f>Miscellaneous[[#This Row],[Budget]]-Miscellaneous[[#This Row],[Actual]]</f>
+        <v>0</v>
+      </c>
+      <c r="O34" s="32"/>
+    </row>
+    <row r="35" spans="2:15" s="48" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="16"/>
+      <c r="C35" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32">
+        <f>Travel[[#This Row],[Budget]]-Travel[[#This Row],[Actual]]</f>
+        <v>0</v>
+      </c>
+      <c r="G35" s="32"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="L35" s="32"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="32">
+        <f>Miscellaneous[[#This Row],[Budget]]-Miscellaneous[[#This Row],[Actual]]</f>
+        <v>0</v>
+      </c>
+      <c r="O35" s="34"/>
+    </row>
+    <row r="36" spans="2:15" s="48" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="16"/>
+      <c r="C36" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="L34" s="32">
-        <f>SUBTOTAL(109,Miscellaneous[Budget])</f>
-        <v>0</v>
-      </c>
-      <c r="M34" s="32">
-        <f>SUBTOTAL(109,Miscellaneous[Actual])</f>
-        <v>0</v>
-      </c>
-      <c r="N34" s="32">
+      <c r="D36" s="32">
+        <f>SUM(Travel[Budget])</f>
+        <v>0</v>
+      </c>
+      <c r="E36" s="32">
+        <f>SUM(Travel[Actual])</f>
+        <v>0</v>
+      </c>
+      <c r="F36" s="32">
+        <f>SUBTOTAL(109,Travel[Difference])</f>
+        <v>0</v>
+      </c>
+      <c r="G36" s="52"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="L36" s="32">
+        <f>SUM(Miscellaneous[Budget])</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="32">
+        <f>SUM(Miscellaneous[Actual])</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="32">
         <f>SUBTOTAL(109,Miscellaneous[Difference])</f>
         <v>0</v>
       </c>
-      <c r="O34" s="52"/>
+      <c r="O36" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="C1:H6"/>
-    <mergeCell ref="K28:N28"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="K30:N30"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="C30:F30"/>
     <mergeCell ref="C9:F9"/>
     <mergeCell ref="K9:N9"/>
-    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="N6:O7">
-    <cfRule type="cellIs" dxfId="0" priority="49" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="49" operator="greaterThan">
       <formula>SUM(N3-N4)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3847,7 +3818,7 @@
   <pageSetup scale="52" orientation="landscape" horizontalDpi="4294967292" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="N15 N20:N26 F20:F25 F30:F31 F33 N11:N13" emptyCellReference="1"/>
+    <ignoredError sqref="N15 N21:N27 F21:F26 F32:F33 F35 N11:N13" emptyCellReference="1"/>
   </ignoredErrors>
   <tableParts count="6">
     <tablePart r:id="rId2"/>
@@ -3877,7 +3848,7 @@
               <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>F11:F17 N11:N17 F20:F27 N20:N27 F30:F34 N30:N34</xm:sqref>
+          <xm:sqref>F11:F18 N11:N18 F21:F29 N21:N29 F32:F36 N32:N36</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -3895,6 +3866,26 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="28" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="60f5a4f2d2b0abadcf532d48ebf9cb71">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dd78129e6a1811f84807ad11c651531" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4206,26 +4197,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{134A9979-A829-40A3-B26B-01CED03CFF30}">
   <ds:schemaRefs>
@@ -4235,6 +4206,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16596A88-1FA2-4A0A-9A1F-7891EA27CF07}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1DDBA422-20F9-4397-91DE-261C512BAFAA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4255,18 +4238,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16596A88-1FA2-4A0A-9A1F-7891EA27CF07}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata"/>
 </file>
</xml_diff>